<commit_message>
FF: Rename and slight changes to form template
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/BigFiveInventory/bigFiveItems.xlsx
+++ b/psychopy/demos/builder/BigFiveInventory/bigFiveItems.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\psychopy\psychopy\demos\builder\BigFiveInventory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53F55682-AD2D-4D40-B32A-68196CFFFCCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82CBF0F7-382E-4229-B550-C83ABF085D96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,7 +136,108 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>OPTIONAL</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">
+If the item is a multiple choice response, what options should be available? These should be a list seperated by commas.
+If the item is free text entry, what text should be displayed before any response?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>OPTIONAL</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">
+If the item is a slider, what ticks should it use? These should be numeric and seperated by commas.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>OPTIONAL</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t xml:space="preserve">
+How should each tick be labeled? This should be a list seperated by commas, of the same length as </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <i/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>ticks</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri Light"/>
+            <family val="2"/>
+            <scheme val="major"/>
+          </rPr>
+          <t>.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -176,7 +277,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -202,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -228,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -254,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -277,107 +378,6 @@
           </rPr>
           <t xml:space="preserve">
 What proportion of the available width should be taken up by the item? Should be a value between 0 and 1.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>OPTIONAL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t xml:space="preserve">
-If the item is a multiple choice response, what options should be available? These should be a list seperated by commas.
-If the item is free text entry, what text should be displayed before any response?</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>OPTIONAL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t xml:space="preserve">
-If the item is a slider, what ticks should it use? These should be numeric and seperated by commas.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>OPTIONAL</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t xml:space="preserve">
-How should each tick be labeled? This should be a list seperated by commas, of the same length as </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <i/>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>ticks</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Calibri Light"/>
-            <family val="2"/>
-            <scheme val="major"/>
-          </rPr>
-          <t>.</t>
         </r>
       </text>
     </comment>
@@ -976,11 +976,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L45"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -988,12 +988,12 @@
     <col min="1" max="1" width="6.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="2" customWidth="1"/>
-    <col min="5" max="8" width="15.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="2" customWidth="1"/>
-    <col min="10" max="11" width="25.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="5" hidden="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4" hidden="1"/>
+    <col min="4" max="4" width="25.7109375" style="2" customWidth="1"/>
+    <col min="5" max="6" width="25.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="2" customWidth="1"/>
+    <col min="8" max="11" width="15.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="4" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="3" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1007,28 +1007,28 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1042,16 +1042,16 @@
         <v>57</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H2" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1065,16 +1065,16 @@
         <v>57</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1088,16 +1088,16 @@
         <v>57</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1111,16 +1111,16 @@
         <v>57</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1134,16 +1134,16 @@
         <v>57</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1157,16 +1157,16 @@
         <v>57</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K7" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1180,16 +1180,16 @@
         <v>57</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1203,16 +1203,16 @@
         <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1226,16 +1226,16 @@
         <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1249,16 +1249,16 @@
         <v>57</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1272,16 +1272,16 @@
         <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H12" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1295,16 +1295,16 @@
         <v>57</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H13" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K13" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1318,16 +1318,16 @@
         <v>57</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H14" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K14" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1341,16 +1341,16 @@
         <v>57</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H15" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -1364,19 +1364,19 @@
         <v>57</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H16" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1387,19 +1387,19 @@
         <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H17" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1410,19 +1410,19 @@
         <v>57</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1433,19 +1433,19 @@
         <v>57</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1456,19 +1456,19 @@
         <v>57</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F20" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H20" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K20" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1479,19 +1479,19 @@
         <v>57</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H21" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K21" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1502,19 +1502,19 @@
         <v>57</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1525,19 +1525,19 @@
         <v>57</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F23" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1548,19 +1548,19 @@
         <v>57</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1571,19 +1571,19 @@
         <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H25" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -1594,19 +1594,19 @@
         <v>57</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H26" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K26" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -1617,19 +1617,19 @@
         <v>57</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F27" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H27" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K27" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -1640,19 +1640,19 @@
         <v>57</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F28" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H28" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K28" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -1663,19 +1663,19 @@
         <v>57</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F29" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H29" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -1686,19 +1686,19 @@
         <v>57</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F30" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H30" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K30" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -1709,19 +1709,19 @@
         <v>57</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F31" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H31" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -1732,19 +1732,19 @@
         <v>57</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F32" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H32" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K32" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -1755,19 +1755,19 @@
         <v>57</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F33" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H33" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I33" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -1778,19 +1778,19 @@
         <v>57</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F34" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H34" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I34" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K34" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -1801,19 +1801,19 @@
         <v>57</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H35" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I35" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K35" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -1824,19 +1824,19 @@
         <v>57</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F36" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K36" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -1847,19 +1847,19 @@
         <v>57</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F37" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I37" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K37" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -1870,19 +1870,19 @@
         <v>57</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F38" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H38" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I38" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1893,19 +1893,19 @@
         <v>57</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F39" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H39" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I39" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1916,19 +1916,19 @@
         <v>57</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H40" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I40" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -1939,19 +1939,19 @@
         <v>57</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H41" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -1962,19 +1962,19 @@
         <v>57</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F42" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H42" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -1985,19 +1985,19 @@
         <v>57</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F43" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H43" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I43" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2008,19 +2008,19 @@
         <v>57</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F44" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H44" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I44" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2031,16 +2031,16 @@
         <v>57</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="F45" s="1">
-        <v>0.6</v>
-      </c>
-      <c r="H45" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>55</v>
+        <v>55</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I45" s="1">
+        <v>0.6</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>